<commit_message>
Format all install numbers like integers (instead of strings with commas)
</commit_message>
<xml_diff>
--- a/data/cleaned/health_and_fitness_apps.xlsx
+++ b/data/cleaned/health_and_fitness_apps.xlsx
@@ -616,10 +616,8 @@
           <t>Want to take charge of your health? Let Google Fit help you reach your goals.</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>100,000,000+</t>
-        </is>
+      <c r="D2" t="n">
+        <v>100000000</v>
       </c>
       <c r="E2" t="n">
         <v>100000000</v>
@@ -757,10 +755,8 @@
           <t>Lifestyle companion to track your fitness, weight, diet, food &amp; sleep.</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>1,000,000,000+</t>
-        </is>
+      <c r="D3" t="n">
+        <v>1000000000</v>
       </c>
       <c r="E3" t="n">
         <v>1000000000</v>
@@ -898,10 +894,8 @@
           <t>Fitbit is dedicated to helping people lead healthier, more active lives.</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>100,000,000+</t>
-        </is>
+      <c r="D4" t="n">
+        <v>100000000</v>
       </c>
       <c r="E4" t="n">
         <v>100000000</v>
@@ -1043,10 +1037,8 @@
           <t>Log food, nutrition, and macros, find high-protein recipes, and lose weight</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>100,000,000+</t>
-        </is>
+      <c r="D5" t="n">
+        <v>100000000</v>
       </c>
       <c r="E5" t="n">
         <v>100000000</v>
@@ -1188,10 +1180,8 @@
           <t>Track your active life in one place and share the journey with friends.</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>50,000,000+</t>
-        </is>
+      <c r="D6" t="n">
+        <v>50000000</v>
       </c>
       <c r="E6" t="n">
         <v>50000000</v>
@@ -1333,10 +1323,8 @@
           <t>Home workouts for fitness &amp; fast bodybuilding at home - no equipment needed.</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>100,000,000+</t>
-        </is>
+      <c r="D7" t="n">
+        <v>100000000</v>
       </c>
       <c r="E7" t="n">
         <v>100000000</v>
@@ -1478,10 +1466,8 @@
           <t>Walking app for weight loss: walk &amp; step counter, pedometer, indoor walking app</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>10,000,000+</t>
-        </is>
+      <c r="D8" t="n">
+        <v>10000000</v>
       </c>
       <c r="E8" t="n">
         <v>10000000</v>
@@ -1623,10 +1609,8 @@
           <t>Sweat and get fit with HIIT, barre, cardio, yoga &amp; more</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>5,000,000+</t>
-        </is>
+      <c r="D9" t="n">
+        <v>5000000</v>
       </c>
       <c r="E9" t="n">
         <v>5000000</v>
@@ -1768,10 +1752,8 @@
           <t>Gym &amp; home workout plans with strength training, exercise tracking, HIIT &amp; more.</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>1,000,000+</t>
-        </is>
+      <c r="D10" t="n">
+        <v>1000000</v>
       </c>
       <c r="E10" t="n">
         <v>1000000</v>
@@ -1913,10 +1895,8 @@
           <t>Gym Log &amp; Workout Tracker | Fitness Journal, Training &amp; Weight Lifting Planner</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>1,000,000+</t>
-        </is>
+      <c r="D11" t="n">
+        <v>1000000</v>
       </c>
       <c r="E11" t="n">
         <v>1000000</v>
@@ -2058,10 +2038,8 @@
           <t>Health &amp; Fitness coaching. Science backed sustainable Nutrition &amp; Training plans</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>1,000,000+</t>
-        </is>
+      <c r="D12" t="n">
+        <v>1000000</v>
       </c>
       <c r="E12" t="n">
         <v>1000000</v>
@@ -2203,10 +2181,8 @@
           <t>A simple way to share data between health, fitness, and wellbeing apps</t>
         </is>
       </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>500,000,000+</t>
-        </is>
+      <c r="D13" t="n">
+        <v>500000000</v>
       </c>
       <c r="E13" t="n">
         <v>500000000</v>
@@ -2344,10 +2320,8 @@
           <t>Workouts for everyone</t>
         </is>
       </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>10,000,000+</t>
-        </is>
+      <c r="D14" t="n">
+        <v>10000000</v>
       </c>
       <c r="E14" t="n">
         <v>10000000</v>
@@ -2489,10 +2463,8 @@
           <t>Meal Planning, Workout Suggestions, AI based Photo Tracking, Calorie Tracking</t>
         </is>
       </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>10,000,000+</t>
-        </is>
+      <c r="D15" t="n">
+        <v>10000000</v>
       </c>
       <c r="E15" t="n">
         <v>10000000</v>
@@ -2634,10 +2606,8 @@
           <t>Achieve your fitness goals: Strength, cardio &amp; ab workouts at the gym or at home</t>
         </is>
       </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>1,000,000+</t>
-        </is>
+      <c r="D16" t="n">
+        <v>1000000</v>
       </c>
       <c r="E16" t="n">
         <v>1000000</v>
@@ -2779,10 +2749,8 @@
           <t>Weight Loss and Better Health</t>
         </is>
       </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>10,000,000+</t>
-        </is>
+      <c r="D17" t="n">
+        <v>10000000</v>
       </c>
       <c r="E17" t="n">
         <v>10000000</v>
@@ -2924,10 +2892,8 @@
           <t>Pilates, Calisthenics, Somatic, Fasting</t>
         </is>
       </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>10,000,000+</t>
-        </is>
+      <c r="D18" t="n">
+        <v>10000000</v>
       </c>
       <c r="E18" t="n">
         <v>10000000</v>
@@ -3069,10 +3035,8 @@
           <t>Quick bodyweight HIIT workouts, just 7 minutes a day!</t>
         </is>
       </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>10,000,000+</t>
-        </is>
+      <c r="D19" t="n">
+        <v>10000000</v>
       </c>
       <c r="E19" t="n">
         <v>10000000</v>
@@ -3214,10 +3178,8 @@
           <t>Home routines, bodybuilding tracker. Personal trainer, coach. Exercise for women</t>
         </is>
       </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>5,000,000+</t>
-        </is>
+      <c r="D20" t="n">
+        <v>5000000</v>
       </c>
       <c r="E20" t="n">
         <v>5000000</v>
@@ -3359,10 +3321,8 @@
           <t>Elevate your health and wellness journey with NTC. Workouts, mindfulness &amp; more.</t>
         </is>
       </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>10,000,000+</t>
-        </is>
+      <c r="D21" t="n">
+        <v>10000000</v>
       </c>
       <c r="E21" t="n">
         <v>10000000</v>
@@ -3500,10 +3460,8 @@
           <t>Daily step tracker, free pedometer &amp; map tracker to count steps and calories.</t>
         </is>
       </c>
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>10,000,000+</t>
-        </is>
+      <c r="D22" t="n">
+        <v>10000000</v>
       </c>
       <c r="E22" t="n">
         <v>10000000</v>
@@ -3645,10 +3603,8 @@
           <t>Mood journal, habits, self-care tracker, self-love</t>
         </is>
       </c>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>5,000,000+</t>
-        </is>
+      <c r="D23" t="n">
+        <v>5000000</v>
       </c>
       <c r="E23" t="n">
         <v>5000000</v>
@@ -3790,10 +3746,8 @@
           <t>Create workout plans for the gym or home with our customizable workout planner</t>
         </is>
       </c>
-      <c r="D24" t="inlineStr">
-        <is>
-          <t>10,000,000+</t>
-        </is>
+      <c r="D24" t="n">
+        <v>10000000</v>
       </c>
       <c r="E24" t="n">
         <v>10000000</v>
@@ -3935,10 +3889,8 @@
           <t>Home &amp; gym workouts for you, Video library. Track progress effortlessly!</t>
         </is>
       </c>
-      <c r="D25" t="inlineStr">
-        <is>
-          <t>5,000,000+</t>
-        </is>
+      <c r="D25" t="n">
+        <v>5000000</v>
       </c>
       <c r="E25" t="n">
         <v>5000000</v>
@@ -4080,10 +4032,8 @@
           <t>Build muscle with JEFIT: Gym workout app with plan/track/sync tools. Free!</t>
         </is>
       </c>
-      <c r="D26" t="inlineStr">
-        <is>
-          <t>5,000,000+</t>
-        </is>
+      <c r="D26" t="n">
+        <v>5000000</v>
       </c>
       <c r="E26" t="n">
         <v>5000000</v>
@@ -4225,10 +4175,8 @@
           <t>Looking to take control of your health? Our psychology-based programs can help.</t>
         </is>
       </c>
-      <c r="D27" t="inlineStr">
-        <is>
-          <t>10,000,000+</t>
-        </is>
+      <c r="D27" t="n">
+        <v>10000000</v>
       </c>
       <c r="E27" t="n">
         <v>10000000</v>
@@ -4370,10 +4318,8 @@
           <t>Lose weight &amp; reach your health goals with Lose It! diet app and food tracker!</t>
         </is>
       </c>
-      <c r="D28" t="inlineStr">
-        <is>
-          <t>10,000,000+</t>
-        </is>
+      <c r="D28" t="n">
+        <v>10000000</v>
       </c>
       <c r="E28" t="n">
         <v>10000000</v>
@@ -4515,10 +4461,8 @@
           <t>Tackle everyday stress and anxiety. Self-care and sound sleep through meditation</t>
         </is>
       </c>
-      <c r="D29" t="inlineStr">
-        <is>
-          <t>50,000,000+</t>
-        </is>
+      <c r="D29" t="n">
+        <v>50000000</v>
       </c>
       <c r="E29" t="n">
         <v>50000000</v>
@@ -4660,10 +4604,8 @@
           <t>Explore the outdoors: hiking trail maps, bike trails, camping &amp; backpacking maps</t>
         </is>
       </c>
-      <c r="D30" t="inlineStr">
-        <is>
-          <t>10,000,000+</t>
-        </is>
+      <c r="D30" t="n">
+        <v>10000000</v>
       </c>
       <c r="E30" t="n">
         <v>10000000</v>
@@ -4805,10 +4747,8 @@
           <t>A personal trainer in your pocket. At-home HIIT workouts &amp; custom training plans</t>
         </is>
       </c>
-      <c r="D31" t="inlineStr">
-        <is>
-          <t>10,000,000+</t>
-        </is>
+      <c r="D31" t="n">
+        <v>10000000</v>
       </c>
       <c r="E31" t="n">
         <v>10000000</v>

</xml_diff>